<commit_message>
Added Team, TeamDetails, UserActivities & CommonType Collection | CRUD Ops for Teams Created
</commit_message>
<xml_diff>
--- a/Functionality & Table Structure.xlsx
+++ b/Functionality & Table Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tejas\OneDrive\Desktop\Desktop Files\Website Development\Project TeamLabs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tejas\OneDrive\Desktop\Desktop Files\Website Development\Project TeamLabs\code_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD412A9-E8D6-4E73-A916-42C720A22191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA037532-28F3-4EF3-8768-CFF62C3885C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D8E241EB-A419-4EEE-B392-5A3A105D9CF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D8E241EB-A419-4EEE-B392-5A3A105D9CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Functionalities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="116">
   <si>
     <t>Functionality</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Deployment</t>
   </si>
   <si>
-    <t>Teams</t>
-  </si>
-  <si>
     <r>
       <t>/API/Teams/UpdateMemberDetailsForTeam?</t>
     </r>
@@ -755,6 +752,15 @@
       </rPr>
       <t>=101</t>
     </r>
+  </si>
+  <si>
+    <t>TeamType</t>
+  </si>
+  <si>
+    <t>Service Integration</t>
+  </si>
+  <si>
+    <t>InHouse</t>
   </si>
 </sst>
 </file>
@@ -798,7 +804,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -858,11 +864,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -931,6 +974,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,9 +1001,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -989,7 +1041,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1095,7 +1147,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1237,7 +1289,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1418,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC9AB8C-15A7-4D62-89DB-BDBA00BF1F7D}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:K13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K39" sqref="A1:K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,8 +1723,8 @@
       <c r="J10" s="5">
         <v>1</v>
       </c>
-      <c r="K10" s="19" t="s">
-        <v>97</v>
+      <c r="K10" s="24" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1689,7 +1741,7 @@
       <c r="J11" s="5">
         <v>2</v>
       </c>
-      <c r="K11" s="19"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E12" s="3" t="s">
@@ -1705,7 +1757,7 @@
       <c r="J12" s="5">
         <v>3</v>
       </c>
-      <c r="K12" s="19"/>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E13" s="3" t="s">
@@ -1721,7 +1773,7 @@
       <c r="J13" s="5">
         <v>4</v>
       </c>
-      <c r="K13" s="19"/>
+      <c r="K13" s="25"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E14" s="3" t="s">
@@ -1731,6 +1783,22 @@
         <v>33</v>
       </c>
       <c r="G14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" s="5">
+        <v>5</v>
+      </c>
+      <c r="K14" s="25"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="5">
+        <v>6</v>
+      </c>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
@@ -2121,7 +2189,6 @@
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="K5:K9"/>
-    <mergeCell ref="K10:K13"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="A26:C26"/>
@@ -2130,6 +2197,7 @@
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="E26:G26"/>
+    <mergeCell ref="K10:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2139,7 +2207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E24B35B-9ECB-4DE8-9425-9B90F3EBFB7D}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2155,7 +2223,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>21</v>
@@ -2166,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>90</v>
@@ -2177,7 +2245,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>89</v>
@@ -2188,7 +2256,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>89</v>
@@ -2199,7 +2267,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>91</v>
@@ -2215,7 +2283,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>21</v>
@@ -2259,7 +2327,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>91</v>
@@ -2270,7 +2338,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>21</v>
@@ -2292,7 +2360,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>90</v>
@@ -2303,7 +2371,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>90</v>
@@ -2314,7 +2382,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>91</v>
@@ -2325,7 +2393,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>90</v>
@@ -2336,7 +2404,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>89</v>
@@ -2347,7 +2415,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>89</v>
@@ -2358,7 +2426,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>89</v>
@@ -2369,7 +2437,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Completed CRUD Operations on a Project | Adding & Removing a Team to the Project | Granting or Revoking Access of a Project Resources to a Team.
</commit_message>
<xml_diff>
--- a/Functionality & Table Structure.xlsx
+++ b/Functionality & Table Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tejas\OneDrive\Desktop\Desktop Files\Website Development\Project TeamLabs\code_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA037532-28F3-4EF3-8768-CFF62C3885C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD1EE4D-8AB4-4794-912A-623295BE8247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D8E241EB-A419-4EEE-B392-5A3A105D9CF0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="115">
   <si>
     <t>Functionality</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>tblProjects</t>
-  </si>
-  <si>
     <t>ProjectID</t>
   </si>
   <si>
@@ -152,12 +149,6 @@
     <t>GUID</t>
   </si>
   <si>
-    <t>OrganisationID_FK</t>
-  </si>
-  <si>
-    <t>tblOrganisations_FK_OrganisationID</t>
-  </si>
-  <si>
     <t>ProjectType</t>
   </si>
   <si>
@@ -761,6 +752,12 @@
   </si>
   <si>
     <t>InHouse</t>
+  </si>
+  <si>
+    <t>ProjectsDetails</t>
+  </si>
+  <si>
+    <t>Projects</t>
   </si>
 </sst>
 </file>
@@ -1470,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC9AB8C-15A7-4D62-89DB-BDBA00BF1F7D}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K39" sqref="A1:K39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K37" sqref="E1:K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,28 +1478,28 @@
     <col min="3" max="3" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="13"/>
     <col min="5" max="5" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="13" customWidth="1"/>
     <col min="7" max="7" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="13"/>
     <col min="9" max="9" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="23"/>
       <c r="E1" s="21" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="23"/>
       <c r="I1" s="20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -1515,7 +1512,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>20</v>
@@ -1524,62 +1521,60 @@
         <v>21</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="C3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J3" s="5">
         <v>0</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>39</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J4" s="5">
         <v>1</v>
@@ -1588,48 +1583,48 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J5" s="5">
         <v>1</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5"/>
       <c r="E6" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J6" s="5">
         <v>2</v>
@@ -1638,23 +1633,21 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5"/>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J7" s="5">
         <v>3</v>
@@ -1663,21 +1656,21 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="5"/>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="E8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="G8" s="5"/>
       <c r="I8" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J8" s="5">
         <v>4</v>
@@ -1686,23 +1679,21 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="5" t="s">
         <v>58</v>
       </c>
+      <c r="F9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J9" s="5">
         <v>5</v>
@@ -1714,29 +1705,29 @@
         <v>25</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J10" s="5">
         <v>1</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E11" s="3" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J11" s="5">
         <v>2</v>
@@ -1745,14 +1736,14 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E12" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J12" s="5">
         <v>3</v>
@@ -1760,15 +1751,8 @@
       <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J13" s="5">
         <v>4</v>
@@ -1776,15 +1760,13 @@
       <c r="K13" s="25"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="5"/>
+      <c r="E14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
       <c r="I14" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J14" s="5">
         <v>5</v>
@@ -1792,8 +1774,17 @@
       <c r="K14" s="25"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="I15" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J15" s="5">
         <v>6</v>
@@ -1802,17 +1793,19 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B16" s="22"/>
       <c r="C16" s="23"/>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
@@ -1820,145 +1813,203 @@
         <v>21</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="5"/>
       <c r="E18" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="5"/>
       <c r="E19" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="I19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" s="5"/>
       <c r="E20" s="3" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="5"/>
       <c r="E21" s="3" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="5"/>
       <c r="E22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="I22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="C23" s="5"/>
-      <c r="E23" s="3" t="s">
+      <c r="I23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="E24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+      <c r="I24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
-      <c r="E26" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>20</v>
       </c>
@@ -1966,228 +2017,212 @@
         <v>21</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="5"/>
       <c r="E28" s="3" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="E29" s="3" t="s">
-        <v>24</v>
+      <c r="E29" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C30" s="5"/>
       <c r="E30" s="3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="E31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="E31" s="10" t="s">
-        <v>81</v>
-      </c>
       <c r="F31" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C32" s="5"/>
       <c r="E32" s="3" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="5"/>
       <c r="E36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="B37" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" s="5"/>
       <c r="E37" s="3" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>82</v>
+        <v>32</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="E38" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="K5:K9"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="K3:K4"/>
@@ -2195,9 +2230,10 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E24:G24"/>
     <mergeCell ref="K10:K15"/>
+    <mergeCell ref="I17:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2223,7 +2259,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>21</v>
@@ -2234,10 +2270,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2245,10 +2281,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2256,10 +2292,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2267,10 +2303,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2283,7 +2319,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>21</v>
@@ -2294,10 +2330,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2305,10 +2341,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2316,10 +2352,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2327,10 +2363,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2338,7 +2374,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>21</v>
@@ -2349,10 +2385,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2360,10 +2396,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2371,10 +2407,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2382,10 +2418,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2393,10 +2429,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2404,10 +2440,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2415,10 +2451,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2426,10 +2462,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2437,10 +2473,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>